<commit_message>
new sample files, long enough
</commit_message>
<xml_diff>
--- a/xls/G1_LP_A.xlsx
+++ b/xls/G1_LP_A.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="13">
   <si>
     <t>pe</t>
   </si>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +644,1482 @@
         <v>31</v>
       </c>
       <c r="M6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>21</v>
+      </c>
+      <c r="K7">
+        <v>22</v>
+      </c>
+      <c r="L7">
+        <v>31</v>
+      </c>
+      <c r="M7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>21</v>
+      </c>
+      <c r="K8">
+        <v>22</v>
+      </c>
+      <c r="L8">
+        <v>31</v>
+      </c>
+      <c r="M8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>11</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>21</v>
+      </c>
+      <c r="K9">
+        <v>22</v>
+      </c>
+      <c r="L9">
+        <v>31</v>
+      </c>
+      <c r="M9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>11</v>
+      </c>
+      <c r="I10">
+        <v>12</v>
+      </c>
+      <c r="J10">
+        <v>21</v>
+      </c>
+      <c r="K10">
+        <v>22</v>
+      </c>
+      <c r="L10">
+        <v>31</v>
+      </c>
+      <c r="M10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="I11">
+        <v>12</v>
+      </c>
+      <c r="J11">
+        <v>21</v>
+      </c>
+      <c r="K11">
+        <v>22</v>
+      </c>
+      <c r="L11">
+        <v>31</v>
+      </c>
+      <c r="M11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>12</v>
+      </c>
+      <c r="J12">
+        <v>21</v>
+      </c>
+      <c r="K12">
+        <v>22</v>
+      </c>
+      <c r="L12">
+        <v>31</v>
+      </c>
+      <c r="M12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>21</v>
+      </c>
+      <c r="K13">
+        <v>22</v>
+      </c>
+      <c r="L13">
+        <v>31</v>
+      </c>
+      <c r="M13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>11</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <v>21</v>
+      </c>
+      <c r="K14">
+        <v>22</v>
+      </c>
+      <c r="L14">
+        <v>31</v>
+      </c>
+      <c r="M14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>21</v>
+      </c>
+      <c r="K15">
+        <v>22</v>
+      </c>
+      <c r="L15">
+        <v>31</v>
+      </c>
+      <c r="M15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16">
+        <v>11</v>
+      </c>
+      <c r="I16">
+        <v>12</v>
+      </c>
+      <c r="J16">
+        <v>21</v>
+      </c>
+      <c r="K16">
+        <v>22</v>
+      </c>
+      <c r="L16">
+        <v>31</v>
+      </c>
+      <c r="M16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>11</v>
+      </c>
+      <c r="I17">
+        <v>12</v>
+      </c>
+      <c r="J17">
+        <v>21</v>
+      </c>
+      <c r="K17">
+        <v>22</v>
+      </c>
+      <c r="L17">
+        <v>31</v>
+      </c>
+      <c r="M17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18">
+        <v>11</v>
+      </c>
+      <c r="I18">
+        <v>12</v>
+      </c>
+      <c r="J18">
+        <v>21</v>
+      </c>
+      <c r="K18">
+        <v>22</v>
+      </c>
+      <c r="L18">
+        <v>31</v>
+      </c>
+      <c r="M18">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <v>11</v>
+      </c>
+      <c r="I19">
+        <v>12</v>
+      </c>
+      <c r="J19">
+        <v>21</v>
+      </c>
+      <c r="K19">
+        <v>22</v>
+      </c>
+      <c r="L19">
+        <v>31</v>
+      </c>
+      <c r="M19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <v>11</v>
+      </c>
+      <c r="I20">
+        <v>12</v>
+      </c>
+      <c r="J20">
+        <v>21</v>
+      </c>
+      <c r="K20">
+        <v>22</v>
+      </c>
+      <c r="L20">
+        <v>31</v>
+      </c>
+      <c r="M20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21">
+        <v>11</v>
+      </c>
+      <c r="I21">
+        <v>12</v>
+      </c>
+      <c r="J21">
+        <v>21</v>
+      </c>
+      <c r="K21">
+        <v>22</v>
+      </c>
+      <c r="L21">
+        <v>31</v>
+      </c>
+      <c r="M21">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22">
+        <v>11</v>
+      </c>
+      <c r="I22">
+        <v>12</v>
+      </c>
+      <c r="J22">
+        <v>21</v>
+      </c>
+      <c r="K22">
+        <v>22</v>
+      </c>
+      <c r="L22">
+        <v>31</v>
+      </c>
+      <c r="M22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <v>12</v>
+      </c>
+      <c r="J23">
+        <v>21</v>
+      </c>
+      <c r="K23">
+        <v>22</v>
+      </c>
+      <c r="L23">
+        <v>31</v>
+      </c>
+      <c r="M23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>11</v>
+      </c>
+      <c r="I24">
+        <v>12</v>
+      </c>
+      <c r="J24">
+        <v>21</v>
+      </c>
+      <c r="K24">
+        <v>22</v>
+      </c>
+      <c r="L24">
+        <v>31</v>
+      </c>
+      <c r="M24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25">
+        <v>11</v>
+      </c>
+      <c r="I25">
+        <v>12</v>
+      </c>
+      <c r="J25">
+        <v>21</v>
+      </c>
+      <c r="K25">
+        <v>22</v>
+      </c>
+      <c r="L25">
+        <v>31</v>
+      </c>
+      <c r="M25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26">
+        <v>11</v>
+      </c>
+      <c r="I26">
+        <v>12</v>
+      </c>
+      <c r="J26">
+        <v>21</v>
+      </c>
+      <c r="K26">
+        <v>22</v>
+      </c>
+      <c r="L26">
+        <v>31</v>
+      </c>
+      <c r="M26">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27">
+        <v>11</v>
+      </c>
+      <c r="I27">
+        <v>12</v>
+      </c>
+      <c r="J27">
+        <v>21</v>
+      </c>
+      <c r="K27">
+        <v>22</v>
+      </c>
+      <c r="L27">
+        <v>31</v>
+      </c>
+      <c r="M27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28">
+        <v>11</v>
+      </c>
+      <c r="I28">
+        <v>12</v>
+      </c>
+      <c r="J28">
+        <v>21</v>
+      </c>
+      <c r="K28">
+        <v>22</v>
+      </c>
+      <c r="L28">
+        <v>31</v>
+      </c>
+      <c r="M28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29">
+        <v>11</v>
+      </c>
+      <c r="I29">
+        <v>12</v>
+      </c>
+      <c r="J29">
+        <v>21</v>
+      </c>
+      <c r="K29">
+        <v>22</v>
+      </c>
+      <c r="L29">
+        <v>31</v>
+      </c>
+      <c r="M29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30">
+        <v>11</v>
+      </c>
+      <c r="I30">
+        <v>12</v>
+      </c>
+      <c r="J30">
+        <v>21</v>
+      </c>
+      <c r="K30">
+        <v>22</v>
+      </c>
+      <c r="L30">
+        <v>31</v>
+      </c>
+      <c r="M30">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31">
+        <v>11</v>
+      </c>
+      <c r="I31">
+        <v>12</v>
+      </c>
+      <c r="J31">
+        <v>21</v>
+      </c>
+      <c r="K31">
+        <v>22</v>
+      </c>
+      <c r="L31">
+        <v>31</v>
+      </c>
+      <c r="M31">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32">
+        <v>11</v>
+      </c>
+      <c r="I32">
+        <v>12</v>
+      </c>
+      <c r="J32">
+        <v>21</v>
+      </c>
+      <c r="K32">
+        <v>22</v>
+      </c>
+      <c r="L32">
+        <v>31</v>
+      </c>
+      <c r="M32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33">
+        <v>11</v>
+      </c>
+      <c r="I33">
+        <v>12</v>
+      </c>
+      <c r="J33">
+        <v>21</v>
+      </c>
+      <c r="K33">
+        <v>22</v>
+      </c>
+      <c r="L33">
+        <v>31</v>
+      </c>
+      <c r="M33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34">
+        <v>11</v>
+      </c>
+      <c r="I34">
+        <v>12</v>
+      </c>
+      <c r="J34">
+        <v>21</v>
+      </c>
+      <c r="K34">
+        <v>22</v>
+      </c>
+      <c r="L34">
+        <v>31</v>
+      </c>
+      <c r="M34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35">
+        <v>11</v>
+      </c>
+      <c r="I35">
+        <v>12</v>
+      </c>
+      <c r="J35">
+        <v>21</v>
+      </c>
+      <c r="K35">
+        <v>22</v>
+      </c>
+      <c r="L35">
+        <v>31</v>
+      </c>
+      <c r="M35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36">
+        <v>11</v>
+      </c>
+      <c r="I36">
+        <v>12</v>
+      </c>
+      <c r="J36">
+        <v>21</v>
+      </c>
+      <c r="K36">
+        <v>22</v>
+      </c>
+      <c r="L36">
+        <v>31</v>
+      </c>
+      <c r="M36">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <v>11</v>
+      </c>
+      <c r="I37">
+        <v>12</v>
+      </c>
+      <c r="J37">
+        <v>21</v>
+      </c>
+      <c r="K37">
+        <v>22</v>
+      </c>
+      <c r="L37">
+        <v>31</v>
+      </c>
+      <c r="M37">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38">
+        <v>11</v>
+      </c>
+      <c r="I38">
+        <v>12</v>
+      </c>
+      <c r="J38">
+        <v>21</v>
+      </c>
+      <c r="K38">
+        <v>22</v>
+      </c>
+      <c r="L38">
+        <v>31</v>
+      </c>
+      <c r="M38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>89</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39">
+        <v>11</v>
+      </c>
+      <c r="I39">
+        <v>12</v>
+      </c>
+      <c r="J39">
+        <v>21</v>
+      </c>
+      <c r="K39">
+        <v>22</v>
+      </c>
+      <c r="L39">
+        <v>31</v>
+      </c>
+      <c r="M39">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40">
+        <v>11</v>
+      </c>
+      <c r="I40">
+        <v>12</v>
+      </c>
+      <c r="J40">
+        <v>21</v>
+      </c>
+      <c r="K40">
+        <v>22</v>
+      </c>
+      <c r="L40">
+        <v>31</v>
+      </c>
+      <c r="M40">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41">
+        <v>11</v>
+      </c>
+      <c r="I41">
+        <v>12</v>
+      </c>
+      <c r="J41">
+        <v>21</v>
+      </c>
+      <c r="K41">
+        <v>22</v>
+      </c>
+      <c r="L41">
+        <v>31</v>
+      </c>
+      <c r="M41">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42">
+        <v>11</v>
+      </c>
+      <c r="I42">
+        <v>12</v>
+      </c>
+      <c r="J42">
+        <v>21</v>
+      </c>
+      <c r="K42">
+        <v>22</v>
+      </c>
+      <c r="L42">
+        <v>31</v>
+      </c>
+      <c r="M42">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
exchanged LP xls files
</commit_message>
<xml_diff>
--- a/xls/G1_LP_A.xlsx
+++ b/xls/G1_LP_A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="10050"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,45 +16,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="32">
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>fu</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
   <si>
     <t>pe</t>
   </si>
   <si>
-    <t>fi</t>
-  </si>
-  <si>
-    <t>lo</t>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>ta</t>
+  </si>
+  <si>
+    <t>so</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>la</t>
+  </si>
+  <si>
+    <t>fe</t>
+  </si>
+  <si>
+    <t>ni</t>
+  </si>
+  <si>
+    <t>wa</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>ki</t>
+  </si>
+  <si>
+    <t>te</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>ti</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>po</t>
+  </si>
+  <si>
+    <t>le</t>
   </si>
   <si>
     <t>bo</t>
   </si>
   <si>
-    <t>fu</t>
-  </si>
-  <si>
-    <t>fa</t>
-  </si>
-  <si>
-    <t>ta</t>
-  </si>
-  <si>
-    <t>ki</t>
-  </si>
-  <si>
-    <t>so</t>
-  </si>
-  <si>
-    <t>ne</t>
+    <t>do</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>se</t>
   </si>
   <si>
     <t>to</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>ba</t>
   </si>
 </sst>
 </file>
@@ -393,35 +450,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H1">
         <v>11</v>
@@ -444,25 +501,25 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>11</v>
@@ -485,25 +542,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>11</v>
@@ -526,25 +583,25 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <v>11</v>
@@ -567,25 +624,25 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>11</v>
@@ -608,25 +665,25 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>11</v>
@@ -649,25 +706,25 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <v>11</v>
@@ -690,25 +747,25 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <v>11</v>
@@ -731,25 +788,25 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>11</v>
@@ -772,25 +829,25 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <v>11</v>
@@ -813,25 +870,25 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <v>11</v>
@@ -854,25 +911,25 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <v>11</v>
@@ -895,25 +952,25 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <v>11</v>
@@ -936,25 +993,25 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <v>11</v>
@@ -977,25 +1034,25 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>11</v>
@@ -1018,25 +1075,25 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H16">
         <v>11</v>
@@ -1059,25 +1116,25 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>11</v>
@@ -1100,25 +1157,25 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <v>11</v>
@@ -1141,25 +1198,25 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>11</v>
@@ -1182,25 +1239,25 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>11</v>
@@ -1223,25 +1280,25 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>11</v>
@@ -1264,25 +1321,25 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>11</v>
@@ -1305,25 +1362,25 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>11</v>
@@ -1346,25 +1403,25 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H24">
         <v>11</v>
@@ -1387,25 +1444,25 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H25">
         <v>11</v>
@@ -1428,25 +1485,25 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <v>11</v>
@@ -1469,25 +1526,25 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G27" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H27">
         <v>11</v>
@@ -1510,25 +1567,25 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H28">
         <v>11</v>
@@ -1551,25 +1608,25 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G29" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H29">
         <v>11</v>
@@ -1592,25 +1649,25 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H30">
         <v>11</v>
@@ -1633,25 +1690,25 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H31">
         <v>11</v>
@@ -1674,25 +1731,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H32">
         <v>11</v>
@@ -1715,25 +1772,25 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H33">
         <v>11</v>
@@ -1756,25 +1813,25 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
         <v>30</v>
       </c>
-      <c r="B34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" t="s">
-        <v>10</v>
-      </c>
       <c r="G34" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H34">
         <v>11</v>
@@ -1797,25 +1854,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H35">
         <v>11</v>
@@ -1838,25 +1895,25 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H36">
         <v>11</v>
@@ -1879,25 +1936,25 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H37">
         <v>11</v>
@@ -1920,25 +1977,25 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G38" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H38">
         <v>11</v>
@@ -1961,25 +2018,25 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G39" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H39">
         <v>11</v>
@@ -2002,25 +2059,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H40">
         <v>11</v>
@@ -2038,88 +2095,6 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>48</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41">
-        <v>11</v>
-      </c>
-      <c r="I41">
-        <v>12</v>
-      </c>
-      <c r="J41">
-        <v>21</v>
-      </c>
-      <c r="K41">
-        <v>22</v>
-      </c>
-      <c r="L41">
-        <v>31</v>
-      </c>
-      <c r="M41">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>112</v>
-      </c>
-      <c r="B42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42">
-        <v>11</v>
-      </c>
-      <c r="I42">
-        <v>12</v>
-      </c>
-      <c r="J42">
-        <v>21</v>
-      </c>
-      <c r="K42">
-        <v>22</v>
-      </c>
-      <c r="L42">
-        <v>31</v>
-      </c>
-      <c r="M42">
         <v>32</v>
       </c>
     </row>

</xml_diff>